<commit_message>
Updated Sponsors to be Sources
</commit_message>
<xml_diff>
--- a/Template Spreadsheets/Mobile-Marine-NCEI-PACE-Template.xlsx
+++ b/Template Spreadsheets/Mobile-Marine-NCEI-PACE-Template.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/quca3108/Library/CloudStorage/OneDrive-UCB-O365/Desktop/JSONfiles/Template Spreadsheets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/quca3108/Library/CloudStorage/OneDrive-UCB-O365/Desktop/PACE Templates/Template Spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{569C1870-D5FE-3B46-A3F8-31903CFC4C17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC44D361-A013-494F-A0F5-5594B5895D64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="32360" yWindow="-4860" windowWidth="30240" windowHeight="17200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -49,9 +49,6 @@
     <t>Scientists</t>
   </si>
   <si>
-    <t>Sponsors</t>
-  </si>
-  <si>
     <t>Funders</t>
   </si>
   <si>
@@ -230,6 +227,9 @@
   </si>
   <si>
     <t>File(s)</t>
+  </si>
+  <si>
+    <t>Sources</t>
   </si>
 </sst>
 </file>
@@ -1502,8 +1502,8 @@
   </sheetPr>
   <dimension ref="A1:BR2"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="AR1" workbookViewId="0">
-      <selection activeCell="AU13" sqref="AU13"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1585,7 +1585,7 @@
   <sheetData>
     <row r="1" spans="1:70" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -1615,184 +1615,184 @@
         <v>8</v>
       </c>
       <c r="K1" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="L1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="T1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="U1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="V1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="W1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="X1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="Y1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="Y1" s="2" t="s">
+      <c r="Z1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="Z1" s="2" t="s">
+      <c r="AA1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="AA1" s="2" t="s">
+      <c r="AB1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="AB1" s="2" t="s">
+      <c r="AC1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="AC1" s="2" t="s">
+      <c r="AD1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="AD1" s="2" t="s">
+      <c r="AE1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="AE1" s="2" t="s">
+      <c r="AF1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="AF1" s="2" t="s">
+      <c r="AG1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="AG1" s="2" t="s">
+      <c r="AH1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="AH1" s="2" t="s">
+      <c r="AI1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="AI1" s="2" t="s">
+      <c r="AJ1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="AJ1" s="2" t="s">
+      <c r="AK1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="AK1" s="2" t="s">
+      <c r="AL1" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="AL1" s="2" t="s">
+      <c r="AM1" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="AM1" s="2" t="s">
+      <c r="AN1" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="AN1" s="2" t="s">
+      <c r="AO1" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="AP1" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="AQ1" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AR1" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="AS1" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="AO1" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="AP1" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="AQ1" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="AR1" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="AS1" s="2" t="s">
+      <c r="AT1" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="AT1" s="2" t="s">
+      <c r="AU1" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AU1" s="2" t="s">
+      <c r="AV1" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="AV1" s="2" t="s">
+      <c r="AW1" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="AW1" s="2" t="s">
+      <c r="AX1" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="AX1" s="2" t="s">
+      <c r="AY1" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="AY1" s="2" t="s">
+      <c r="AZ1" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="AZ1" s="2" t="s">
+      <c r="BA1" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="BA1" s="2" t="s">
+      <c r="BB1" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="BB1" s="2" t="s">
+      <c r="BC1" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="BC1" s="2" t="s">
+      <c r="BD1" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="BD1" s="2" t="s">
+      <c r="BE1" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="BE1" s="2" t="s">
+      <c r="BF1" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="BF1" s="2" t="s">
+      <c r="BG1" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="BG1" s="2" t="s">
+      <c r="BH1" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="BH1" s="2" t="s">
+      <c r="BI1" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="BI1" s="2" t="s">
+      <c r="BJ1" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="BJ1" s="2" t="s">
+      <c r="BK1" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="BK1" s="2" t="s">
+      <c r="BL1" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="BL1" s="2" t="s">
+      <c r="BM1" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="BN1" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="BM1" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="BN1" s="2" t="s">
+      <c r="BO1" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="BO1" s="2" t="s">
+      <c r="BP1" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="BP1" s="2" t="s">
-        <v>61</v>
-      </c>
       <c r="BQ1" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="BR1" s="2" t="s">
         <v>63</v>
-      </c>
-      <c r="BR1" s="2" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:70" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">

</xml_diff>